<commit_message>
Changes to be committed: 	modified:   LAB/Assignments/rmcmillan1PHY2049LABMoEPoFSpace.docx 	modified:   LAB/Assignments/rmcmillan1PHY2049LABMoEPoFSpace.pages 	modified:   LAB/Assignments/rmcmillan1PHY2049LABMoEPoFSpace.xlsx 	modified:   LAB/Assignments/rmcmillan1PHY2049LABMoEPoFSpace2.docx
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmillan1PHY2049LABMoEPoFSpace.xlsx
+++ b/LAB/Assignments/rmcmillan1PHY2049LABMoEPoFSpace.xlsx
@@ -386,11 +386,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="417072808"/>
-        <c:axId val="418706992"/>
+        <c:axId val="769856384"/>
+        <c:axId val="769856776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="417072808"/>
+        <c:axId val="769856384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,12 +503,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418706992"/>
+        <c:crossAx val="769856776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="418706992"/>
+        <c:axId val="769856776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -621,7 +621,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417072808"/>
+        <c:crossAx val="769856384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1230,16 +1230,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1527,7 +1527,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new file:   Assignments/rmcmilan1MoEPoFS.xlsx 	modified:   Assignments/rmcmillan1PHY2049LABMoEPoFSpace.xlsx
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmillan1PHY2049LABMoEPoFSpace.xlsx
+++ b/LAB/Assignments/rmcmillan1PHY2049LABMoEPoFSpace.xlsx
@@ -24,15 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>x-axis (X)</t>
+    <t>fit</t>
   </si>
   <si>
-    <t>y-axis (Y)</t>
+    <t>C/(3.14*r*r)</t>
   </si>
   <si>
-    <t>fit</t>
+    <t>1/r</t>
+  </si>
+  <si>
+    <t>x-axis (X) (radius in mm)</t>
+  </si>
+  <si>
+    <t>y-axis (Y) Capacitance in Farads</t>
   </si>
 </sst>
 </file>
@@ -386,11 +392,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="769856384"/>
-        <c:axId val="769856776"/>
+        <c:axId val="398010896"/>
+        <c:axId val="635773464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="769856384"/>
+        <c:axId val="398010896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,7 +437,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>x-axis (X)</a:t>
+                  <a:t>x-axis (X) (radius in mm)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -503,12 +509,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="769856776"/>
+        <c:crossAx val="635773464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="769856776"/>
+        <c:axId val="635773464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +555,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>y-axis (Y)</a:t>
+                  <a:t>y-axis (Y) Capacitance in Farads</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -621,7 +627,319 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="769856384"/>
+        <c:crossAx val="398010896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>14.285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0909090909090917</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3333333333333339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>97.491225789678907</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>149.28343949044583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>176.92852087756546</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210.19108280254773</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>228.9835237142706</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>227.79547062986555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="403171224"/>
+        <c:axId val="403503528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="403171224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403503528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="403503528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403171224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -710,6 +1028,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1226,20 +1584,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>185739</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>309564</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1253,6 +2127,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1524,26 +2428,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>7</v>
       </c>
@@ -1554,48 +2470,96 @@
         <f>$A$12*B2+$B$12</f>
         <v>1.2523809523809515</v>
       </c>
+      <c r="E2">
+        <f>1/(B2/100)</f>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="F2">
+        <f>C2/(3.14*(B2/100)*(B2/100))</f>
+        <v>97.491225789678907</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>8</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="0">1/(B3/100)</f>
+        <v>12.5</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="1">C3/(3.14*(B3/100)*(B3/100))</f>
+        <v>149.28343949044583</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4">
         <v>4.5</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>176.92852087756546</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>10</v>
       </c>
       <c r="C5">
         <v>6.6</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>210.19108280254773</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>11</v>
       </c>
       <c r="C6">
         <v>8.6999999999999993</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090917</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>228.9835237142706</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>12</v>
       </c>
       <c r="C7">
         <v>10.3</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>227.79547062986555</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="array" ref="A12:B16">LINEST(C2:C7,B2:B7,TRUE,TRUE)</f>
         <v>1.8057142857142856</v>
@@ -1604,7 +2568,7 @@
         <v>-11.387619047619047</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6.0090634492751864E-2</v>
       </c>
@@ -1612,7 +2576,7 @@
         <v>0.58001211966381916</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.99558982369265026</v>
       </c>
@@ -1620,7 +2584,7 @@
         <v>0.25137715924577608</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>902.99321778447541</v>
       </c>
@@ -1628,7 +2592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>57.060571428571436</v>
       </c>

</xml_diff>